<commit_message>
Update / Clean up of Dennis Sandbox
Updated Model analysis code
Updated Final Presentation (Results), Reference URLs, Planning Notes
Cleaned out redundant test files
</commit_message>
<xml_diff>
--- a/Planning/DAT 205 Notes.xlsx
+++ b/Planning/DAT 205 Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Data-Den\GitHub\Capstone\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA328E31-757B-407D-ACE2-F5F8B04308AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42FA04-26BB-491D-BF0B-A91815D4FFF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F161B801-F3B1-41BF-9526-2FC287A0F2A4}"/>
   </bookViews>
@@ -573,7 +573,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,8 +621,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,13 +656,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF5B9BD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,13 +727,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -737,12 +753,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -757,6 +767,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2138,10 +2157,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC58182-0F82-4FE8-B6FD-DCCF07510BC2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:I140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2152,2296 +2172,2302 @@
     <col min="4" max="4" width="18.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="33.140625" style="3" customWidth="1"/>
     <col min="6" max="7" width="49.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="12" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
     <col min="10" max="16384" width="13.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
         <v>10127</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>768805383</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>6205</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>12691</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
         <v>12</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5">
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
         <v>0</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5">
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="19">
+      <c r="D13" s="4"/>
+      <c r="E13" s="16">
         <v>0.8833333333333333</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="20">
+      <c r="D14" s="4"/>
+      <c r="E14" s="17">
         <v>0.5</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5">
+      <c r="C19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4">
         <v>-10</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="21"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="G20" s="4"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="21" t="s">
+      <c r="G22" s="4"/>
+      <c r="H22" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5">
+      <c r="C23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4">
         <v>202710</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="21" t="s">
+      <c r="G23" s="4"/>
+      <c r="H23" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="21" t="s">
+      <c r="G24" s="4"/>
+      <c r="H24" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
         <v>1610612741</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="21" t="s">
+      <c r="G25" s="4"/>
+      <c r="H25" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="21" t="s">
+      <c r="G26" s="4"/>
+      <c r="H26" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="21" t="s">
+      <c r="G27" s="4"/>
+      <c r="H27" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="16" t="s">
+      <c r="A29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="21" t="s">
+      <c r="G29" s="4"/>
+      <c r="H29" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="21" t="s">
+      <c r="G31" s="4"/>
+      <c r="H31" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="16" t="s">
+      <c r="A32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4">
         <v>24.25</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="21" t="s">
+      <c r="G32" s="4"/>
+      <c r="H32" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5">
+      <c r="C33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4">
         <v>2</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="21" t="s">
+      <c r="G33" s="4"/>
+      <c r="H33" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5">
+      <c r="C34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4">
         <v>7</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="21" t="s">
+      <c r="G34" s="4"/>
+      <c r="H34" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="21" t="s">
+      <c r="G35" s="4"/>
+      <c r="H35" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5">
+      <c r="C36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4">
         <v>0</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="21" t="s">
+      <c r="G36" s="4"/>
+      <c r="H36" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5">
+      <c r="C37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4">
         <v>0</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="21" t="s">
+      <c r="G37" s="4"/>
+      <c r="H37" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="16" t="s">
+      <c r="A38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4">
         <v>0</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="21" t="s">
+      <c r="G38" s="4"/>
+      <c r="H38" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5">
+      <c r="C39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4">
         <v>0</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="21" t="s">
+      <c r="G39" s="4"/>
+      <c r="H39" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="16" t="s">
+      <c r="A40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5">
+      <c r="C40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4">
         <v>0</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="21" t="s">
+      <c r="G40" s="4"/>
+      <c r="H40" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4">
         <v>0</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="21" t="s">
+      <c r="G41" s="4"/>
+      <c r="H41" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="16" t="s">
+      <c r="A42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5">
+      <c r="C42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4">
         <v>0</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="21" t="s">
+      <c r="G42" s="4"/>
+      <c r="H42" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" s="16" t="s">
+      <c r="A43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5">
+      <c r="C43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4">
         <v>3</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="21" t="s">
+      <c r="G43" s="4"/>
+      <c r="H43" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="16" t="s">
+      <c r="A44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5">
+      <c r="C44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4">
         <v>3</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="21" t="s">
+      <c r="G44" s="4"/>
+      <c r="H44" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="16" t="s">
+      <c r="A45" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5">
-        <v>6</v>
-      </c>
-      <c r="F45" s="5" t="s">
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4">
+        <v>6</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="21" t="s">
+      <c r="G45" s="4"/>
+      <c r="H45" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="16" t="s">
+      <c r="A46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5">
+      <c r="C46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4">
         <v>1</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="21" t="s">
+      <c r="G46" s="4"/>
+      <c r="H46" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="16" t="s">
+      <c r="A47" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5">
+      <c r="C47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4">
         <v>1</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="21" t="s">
+      <c r="G47" s="4"/>
+      <c r="H47" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="16" t="s">
+      <c r="A48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5">
+      <c r="C48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4">
         <v>1</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="21" t="s">
+      <c r="G48" s="4"/>
+      <c r="H48" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="16" t="s">
+      <c r="A49" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5">
+      <c r="C49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4">
         <v>0</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="21" t="s">
+      <c r="G49" s="4"/>
+      <c r="H49" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="16" t="s">
+      <c r="A50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5">
+      <c r="C50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4">
         <v>3</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="21" t="s">
+      <c r="G50" s="4"/>
+      <c r="H50" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="16" t="s">
+      <c r="A51" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5">
+      <c r="C51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4">
         <v>0</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="21" t="s">
+      <c r="G51" s="4"/>
+      <c r="H51" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" s="16" t="s">
+      <c r="A52" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5">
+      <c r="C52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4">
         <v>4</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="21" t="s">
+      <c r="G52" s="4"/>
+      <c r="H52" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="16" t="s">
+      <c r="A53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5">
+      <c r="C53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4">
         <v>11</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="21" t="s">
+      <c r="G53" s="4"/>
+      <c r="H53" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="16" t="s">
+    <row r="54" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5">
+      <c r="C54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4">
         <v>21.6</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="21"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" s="16" t="s">
+      <c r="A55" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5">
+      <c r="C55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4">
         <v>0</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="21" t="s">
+      <c r="G55" s="4"/>
+      <c r="H55" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" s="16" t="s">
+      <c r="A56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5">
+      <c r="C56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4">
         <v>0</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="21" t="s">
+      <c r="G56" s="4"/>
+      <c r="H56" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="16" t="s">
+    <row r="57" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5">
+      <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4">
         <v>1</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="21"/>
-    </row>
-    <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="16" t="s">
+      <c r="G57" s="4"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5">
+      <c r="C58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4">
         <v>1</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="16" t="s">
+      <c r="G58" s="4"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5">
+      <c r="C59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4">
         <v>1</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" s="16" t="s">
+      <c r="G59" s="4"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5">
+      <c r="C60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4">
         <v>1</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="21"/>
-    </row>
-    <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61" s="16" t="s">
+      <c r="G60" s="4"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5">
+      <c r="C61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4">
         <v>690</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" s="16" t="s">
+      <c r="G61" s="4"/>
+      <c r="H61" s="18"/>
+    </row>
+    <row r="62" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5">
+      <c r="C62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4">
         <v>1313</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="21"/>
-    </row>
-    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="16" t="s">
+      <c r="G62" s="4"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5">
+      <c r="C63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4">
         <v>1001</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="21"/>
-    </row>
-    <row r="64" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" s="16" t="s">
+      <c r="G63" s="4"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="64" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5">
+      <c r="C64" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4">
         <v>1918</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="21"/>
-    </row>
-    <row r="65" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B65" s="16" t="s">
+      <c r="G64" s="4"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5">
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4">
         <v>1097</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G65" s="5"/>
-      <c r="H65" s="21"/>
-    </row>
-    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" s="16" t="s">
+      <c r="G65" s="4"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5">
+      <c r="C66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4">
         <v>1850</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="21"/>
-    </row>
-    <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="16" t="s">
+      <c r="G66" s="4"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5">
+      <c r="C67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4">
         <v>1097</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G67" s="5"/>
-      <c r="H67" s="21"/>
-    </row>
-    <row r="68" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B68" s="16" t="s">
+      <c r="G67" s="4"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5">
+      <c r="C68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4">
         <v>1570</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="21"/>
-    </row>
-    <row r="69" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B69" s="16" t="s">
+      <c r="G68" s="4"/>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5">
+      <c r="C69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4">
         <v>1672</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="21"/>
-    </row>
-    <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B70" s="16" t="s">
+      <c r="G69" s="4"/>
+      <c r="H69" s="18"/>
+    </row>
+    <row r="70" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5">
+      <c r="C70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4">
         <v>1570</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G70" s="5"/>
-      <c r="H70" s="21"/>
-    </row>
-    <row r="71" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="16" t="s">
+      <c r="G70" s="4"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5">
+      <c r="C71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4">
         <v>1291</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="21"/>
-    </row>
-    <row r="72" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B72" s="16" t="s">
+      <c r="G71" s="4"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5">
+      <c r="C72" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4">
         <v>824</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="21"/>
-    </row>
-    <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B73" s="16" t="s">
+      <c r="G72" s="4"/>
+      <c r="H72" s="18"/>
+    </row>
+    <row r="73" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5">
+      <c r="C73" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4">
         <v>1161</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="21"/>
-    </row>
-    <row r="74" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B74" s="16" t="s">
+      <c r="G73" s="4"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B74" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5">
+      <c r="C74" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4">
         <v>80</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G74" s="5"/>
-      <c r="H74" s="21"/>
-    </row>
-    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" s="16" t="s">
+      <c r="G74" s="4"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5">
+      <c r="C75" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4">
         <v>985</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G75" s="5"/>
-      <c r="H75" s="21"/>
-    </row>
-    <row r="76" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B76" s="16" t="s">
+      <c r="G75" s="4"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5">
+      <c r="C76" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4">
         <v>438</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G76" s="5"/>
-      <c r="H76" s="21"/>
-    </row>
-    <row r="77" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" s="16" t="s">
+      <c r="G76" s="4"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5">
+      <c r="C77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4">
         <v>217</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G77" s="5"/>
-      <c r="H77" s="21"/>
-    </row>
-    <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B78" s="16" t="s">
+      <c r="G77" s="4"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5">
+      <c r="C78" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4">
         <v>1</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G78" s="5"/>
-      <c r="H78" s="21"/>
-    </row>
-    <row r="79" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B79" s="16" t="s">
+      <c r="G78" s="4"/>
+      <c r="H78" s="18"/>
+    </row>
+    <row r="79" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5">
+      <c r="C79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4">
         <v>2005</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G79" s="5"/>
-      <c r="H79" s="21"/>
-    </row>
-    <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B80" s="16" t="s">
+      <c r="G79" s="4"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5">
+      <c r="C80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4">
         <v>2082</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G80" s="5"/>
-      <c r="H80" s="21"/>
-    </row>
-    <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B81" s="16" t="s">
+      <c r="G80" s="4"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B81" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5">
+      <c r="C81" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4">
         <v>1826</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G81" s="5"/>
-      <c r="H81" s="21"/>
-    </row>
-    <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="16" t="s">
+      <c r="G81" s="4"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5">
+      <c r="C82" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4">
         <v>361</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G82" s="5"/>
-      <c r="H82" s="21"/>
-    </row>
-    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B83" s="16" t="s">
+      <c r="G82" s="4"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5">
+      <c r="C83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4">
         <v>803</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F83" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G83" s="5"/>
-      <c r="H83" s="21"/>
-    </row>
-    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B84" s="16" t="s">
+      <c r="G83" s="4"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C84" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5">
+      <c r="C84" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4">
         <v>87</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G84" s="5"/>
-      <c r="H84" s="21"/>
-    </row>
-    <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B85" s="16" t="s">
+      <c r="G84" s="4"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5">
+      <c r="C85" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4">
         <v>2</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G85" s="5"/>
-      <c r="H85" s="21"/>
-    </row>
-    <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B86" s="16" t="s">
+      <c r="G85" s="4"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86" spans="1:8" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="s">
+      <c r="D86" s="4"/>
+      <c r="E86" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G86" s="5"/>
-      <c r="H86" s="21"/>
-    </row>
-    <row r="87" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+      <c r="G86" s="4"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87" spans="1:8" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5" t="s">
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G87" s="5"/>
-      <c r="H87" s="21"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="18"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="B88" s="16"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="21"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="18"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="21"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="18"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="21"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="18"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="B91" s="16"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="21"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="18"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="B92" s="16"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="21"/>
+      <c r="A92" s="4"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="18"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="21"/>
+      <c r="A93" s="4"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="18"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="B94" s="16"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="21"/>
+      <c r="A94" s="4"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="18"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="21"/>
+      <c r="A95" s="4"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="18"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-      <c r="B96" s="16"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="21"/>
+      <c r="A96" s="4"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="18"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-      <c r="B97" s="16"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="21"/>
+      <c r="A97" s="4"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="18"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="16"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="21"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="18"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="16"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="21"/>
+      <c r="A99" s="4"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="18"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="16"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="21"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="18"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="16"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="21"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="16"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="21"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="18"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="16"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="21"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="18"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
-      <c r="B104" s="16"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="21"/>
+      <c r="A104" s="4"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="18"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="5"/>
-      <c r="B105" s="16"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="21"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="18"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="21"/>
+      <c r="A106" s="4"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="18"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="5"/>
-      <c r="B107" s="16"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="21"/>
+      <c r="A107" s="4"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="18"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="5"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="5"/>
-      <c r="H108" s="21"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="18"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
-      <c r="B109" s="16"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5"/>
-      <c r="H109" s="21"/>
+      <c r="A109" s="4"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="18"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
-      <c r="B110" s="16"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="21"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="18"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5"/>
-      <c r="H111" s="21"/>
+      <c r="A111" s="4"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="18"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="16"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
-      <c r="H112" s="21"/>
+      <c r="A112" s="4"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="18"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="16"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="21"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="18"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="16"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="21"/>
+      <c r="A114" s="4"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="18"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="21"/>
+      <c r="A115" s="4"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="18"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="16"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
-      <c r="H116" s="21"/>
+      <c r="A116" s="4"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="18"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="21"/>
+      <c r="A117" s="4"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="18"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="16"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="21"/>
+      <c r="A118" s="4"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="18"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="16"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="21"/>
+      <c r="A119" s="4"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="18"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="21"/>
+      <c r="A120" s="4"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="18"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="21"/>
+      <c r="A121" s="4"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="18"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="16"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
-      <c r="H122" s="21"/>
+      <c r="A122" s="4"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="18"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="16"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-      <c r="H123" s="21"/>
+      <c r="A123" s="4"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="18"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="5"/>
-      <c r="B124" s="16"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
-      <c r="G124" s="5"/>
-      <c r="H124" s="21"/>
+      <c r="A124" s="4"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="18"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="16"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="5"/>
-      <c r="H125" s="21"/>
+      <c r="A125" s="4"/>
+      <c r="B125" s="21"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="18"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="5"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
-      <c r="H126" s="21"/>
+      <c r="A126" s="4"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="18"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="5"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="5"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="5"/>
-      <c r="H127" s="21"/>
+      <c r="A127" s="4"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="18"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="5"/>
-      <c r="B128" s="16"/>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
-      <c r="G128" s="5"/>
-      <c r="H128" s="21"/>
+      <c r="A128" s="4"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="18"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="5"/>
-      <c r="B129" s="16"/>
-      <c r="C129" s="5"/>
-      <c r="D129" s="5"/>
-      <c r="E129" s="5"/>
-      <c r="F129" s="5"/>
-      <c r="G129" s="5"/>
-      <c r="H129" s="21"/>
+      <c r="A129" s="4"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="18"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="5"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="5"/>
-      <c r="D130" s="5"/>
-      <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
-      <c r="G130" s="5"/>
-      <c r="H130" s="21"/>
+      <c r="A130" s="4"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="18"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="5"/>
-      <c r="B131" s="16"/>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="5"/>
-      <c r="H131" s="21"/>
+      <c r="A131" s="4"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="18"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="5"/>
-      <c r="H132" s="21"/>
+      <c r="A132" s="4"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="18"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="16"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
-      <c r="H133" s="21"/>
+      <c r="A133" s="4"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="18"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="5"/>
-      <c r="B134" s="16"/>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
-      <c r="H134" s="21"/>
+      <c r="A134" s="4"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="18"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="5"/>
-      <c r="B135" s="16"/>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
-      <c r="E135" s="5"/>
-      <c r="F135" s="5"/>
-      <c r="G135" s="5"/>
-      <c r="H135" s="21"/>
+      <c r="A135" s="4"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="18"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="16"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
-      <c r="E136" s="5"/>
-      <c r="F136" s="5"/>
-      <c r="G136" s="5"/>
-      <c r="H136" s="21"/>
+      <c r="A136" s="4"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="18"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="5"/>
-      <c r="B137" s="16"/>
-      <c r="C137" s="5"/>
-      <c r="D137" s="5"/>
-      <c r="E137" s="5"/>
-      <c r="F137" s="5"/>
-      <c r="G137" s="5"/>
-      <c r="H137" s="21"/>
+      <c r="A137" s="4"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="18"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="5"/>
-      <c r="B138" s="16"/>
-      <c r="C138" s="5"/>
-      <c r="D138" s="5"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="5"/>
-      <c r="H138" s="21"/>
+      <c r="A138" s="4"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="18"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="5"/>
-      <c r="B139" s="16"/>
-      <c r="C139" s="5"/>
-      <c r="D139" s="5"/>
-      <c r="E139" s="5"/>
-      <c r="F139" s="5"/>
-      <c r="G139" s="5"/>
-      <c r="H139" s="21"/>
+      <c r="A139" s="4"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+      <c r="G139" s="4"/>
+      <c r="H139" s="18"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" s="5"/>
-      <c r="B140" s="16"/>
-      <c r="C140" s="5"/>
-      <c r="D140" s="5"/>
-      <c r="E140" s="5"/>
-      <c r="F140" s="5"/>
-      <c r="G140" s="5"/>
-      <c r="H140" s="21"/>
+      <c r="A140" s="4"/>
+      <c r="B140" s="21"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H87" xr:uid="{F87E7E9E-720B-4630-B7FB-B32ABEC78BAD}"/>
+  <autoFilter ref="A2:H87" xr:uid="{F87E7E9E-720B-4630-B7FB-B32ABEC78BAD}">
+    <filterColumn colId="7">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -4460,695 +4486,695 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="21" style="9" customWidth="1"/>
-    <col min="3" max="3" width="2.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="2.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="2.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="30" style="9" customWidth="1"/>
-    <col min="11" max="11" width="2.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="2.42578125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="26" style="9" customWidth="1"/>
-    <col min="15" max="15" width="41.85546875" style="9" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="8.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="21" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="30" style="8" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="2.42578125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="26" style="8" customWidth="1"/>
+    <col min="15" max="15" width="41.85546875" style="8" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="7" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="12"/>
+      <c r="B4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="O24" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="25" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="N25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O25" s="9" t="s">
+      <c r="O25" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="N26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="9" t="s">
+      <c r="O26" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="27" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J27" s="6" t="s">
+      <c r="J27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N27" s="9" t="s">
+      <c r="N27" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="O27" s="9" t="s">
+      <c r="O27" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="28" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="6" t="s">
+      <c r="J28" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="O28" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="29" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="6" t="s">
+      <c r="J29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="N29" s="9" t="s">
+      <c r="N29" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O29" s="9" t="s">
+      <c r="O29" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="30" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="6" t="s">
+      <c r="J30" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="N30" s="9" t="s">
+      <c r="N30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="O30" s="9" t="s">
+      <c r="O30" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="31" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O31" s="9" t="s">
+      <c r="O31" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="32" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N32" s="9" t="s">
+      <c r="N32" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="O32" s="9" t="s">
+      <c r="O32" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="33" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N33" s="9" t="s">
+      <c r="N33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="O33" s="9" t="s">
+      <c r="O33" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="34" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N34" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O34" s="9" t="s">
+      <c r="O34" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="35" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N35" s="9" t="s">
+      <c r="N35" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="9" t="s">
+      <c r="O35" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="36" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="O36" s="9" t="s">
+      <c r="O36" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="37" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J37" s="6" t="s">
+      <c r="J37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N37" s="9" t="s">
+      <c r="N37" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="O37" s="9" t="s">
+      <c r="O37" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J38" s="6" t="s">
+      <c r="J38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N38" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="O38" s="9" t="s">
+      <c r="O38" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="39" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J39" s="6" t="s">
+      <c r="J39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="O39" s="9" t="s">
+      <c r="O39" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="40" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N40" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="O40" s="9" t="s">
+      <c r="O40" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="41" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J41" s="6" t="s">
+      <c r="J41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N41" s="9" t="s">
+      <c r="N41" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="O41" s="9" t="s">
+      <c r="O41" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="42" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="6" t="s">
+      <c r="J42" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N42" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="O42" s="9" t="s">
+      <c r="O42" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="43" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J43" s="6" t="s">
+      <c r="J43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N43" s="9" t="s">
+      <c r="N43" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="O43" s="9" t="s">
+      <c r="O43" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="44" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="6" t="s">
+      <c r="J44" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N44" s="9" t="s">
+      <c r="N44" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="O44" s="9" t="s">
+      <c r="O44" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="45" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J45" s="6" t="s">
+      <c r="J45" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N45" s="9" t="s">
+      <c r="N45" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="O45" s="9" t="s">
+      <c r="O45" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="46" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J46" s="6" t="s">
+      <c r="J46" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="N46" s="9" t="s">
+      <c r="N46" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O46" s="9" t="s">
+      <c r="O46" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J47" s="6" t="s">
+      <c r="J47" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="N47" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="O47" s="9" t="s">
+      <c r="O47" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="48" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J48" s="6" t="s">
+      <c r="J48" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N48" s="9" t="s">
+      <c r="N48" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O48" s="9" t="s">
+      <c r="O48" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="49" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J49" s="6" t="s">
+      <c r="J49" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="50" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="6" t="s">
+      <c r="J50" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="51" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J51" s="6" t="s">
+      <c r="J51" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="52" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J52" s="6" t="s">
+      <c r="J52" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="53" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J53" s="6" t="s">
+      <c r="J53" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="54" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J54" s="6" t="s">
+      <c r="J54" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="55" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J55" s="6" t="s">
+      <c r="J55" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="56" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J56" s="6" t="s">
+      <c r="J56" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="57" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J57" s="6" t="s">
+      <c r="J57" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="58" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J58" s="6" t="s">
+      <c r="J58" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="59" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J59" s="6" t="s">
+      <c r="J59" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="60" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J60" s="6" t="s">
+      <c r="J60" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="61" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J61" s="6" t="s">
+      <c r="J61" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="62" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J62" s="6" t="s">
+      <c r="J62" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="63" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J63" s="6" t="s">
+      <c r="J63" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="64" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J64" s="6" t="s">
+      <c r="J64" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="65" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J65" s="6" t="s">
+      <c r="J65" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="66" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J66" s="6" t="s">
+      <c r="J66" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="67" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J67" s="6" t="s">
+      <c r="J67" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="68" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J68" s="6" t="s">
+      <c r="J68" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="69" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J69" s="6" t="s">
+      <c r="J69" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="70" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J70" s="6" t="s">
+      <c r="J70" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="71" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J71" s="6" t="s">
+      <c r="J71" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="72" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J72" s="6" t="s">
+      <c r="J72" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="73" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J73" s="6" t="s">
+      <c r="J73" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="74" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J74" s="6" t="s">
+      <c r="J74" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="75" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J75" s="6" t="s">
+      <c r="J75" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="76" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J76" s="6" t="s">
+      <c r="J76" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="77" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J77" s="6" t="s">
+      <c r="J77" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="78" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J78" s="6" t="s">
+      <c r="J78" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="79" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="6" t="s">
+      <c r="J79" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="80" spans="10:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="6" t="s">
+      <c r="J80" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="81" spans="10:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="6" t="s">
+      <c r="J81" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N81" s="6" t="s">
+      <c r="N81" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O81" s="9" t="s">
+      <c r="O81" s="8" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>